<commit_message>
Experimental results for SBFL only
</commit_message>
<xml_diff>
--- a/experiment_results/SBFL_ONLY/BankAccountTP/1Bug.xlsx
+++ b/experiment_results/SBFL_ONLY/BankAccountTP/1Bug.xlsx
@@ -28,7 +28,7 @@
     <sheet name="Dice" sheetId="19" r:id="rId19"/>
     <sheet name="Humman" sheetId="20" r:id="rId20"/>
     <sheet name="Wong2" sheetId="21" r:id="rId21"/>
-    <sheet name="Wong3" sheetId="22" r:id="rId22"/>
+    <sheet name="Euclid" sheetId="22" r:id="rId22"/>
     <sheet name="Zoltar" sheetId="23" r:id="rId23"/>
     <sheet name="Rogot2" sheetId="24" r:id="rId24"/>
     <sheet name="Hamming" sheetId="25" r:id="rId25"/>
@@ -18511,10 +18511,10 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D2">
-        <v>8.860759493670885</v>
+        <v>25.31645569620253</v>
       </c>
       <c r="E2">
         <v>79</v>
@@ -18528,10 +18528,10 @@
         <v>8</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>68</v>
       </c>
       <c r="D3">
-        <v>3.947368421052631</v>
+        <v>89.47368421052632</v>
       </c>
       <c r="E3">
         <v>76</v>
@@ -18545,10 +18545,10 @@
         <v>10</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D4">
-        <v>2.631578947368421</v>
+        <v>5.263157894736842</v>
       </c>
       <c r="E4">
         <v>76</v>
@@ -18562,10 +18562,10 @@
         <v>12</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="D5">
-        <v>3.947368421052631</v>
+        <v>44.73684210526316</v>
       </c>
       <c r="E5">
         <v>76</v>
@@ -18596,10 +18596,10 @@
         <v>16</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>70</v>
       </c>
       <c r="D7">
-        <v>6.578947368421052</v>
+        <v>92.10526315789474</v>
       </c>
       <c r="E7">
         <v>76</v>
@@ -18613,10 +18613,10 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="D8">
-        <v>12.65822784810127</v>
+        <v>49.36708860759494</v>
       </c>
       <c r="E8">
         <v>79</v>
@@ -18630,10 +18630,10 @@
         <v>19</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="D9">
-        <v>2.631578947368421</v>
+        <v>23.68421052631579</v>
       </c>
       <c r="E9">
         <v>76</v>
@@ -18664,10 +18664,10 @@
         <v>23</v>
       </c>
       <c r="C11">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="D11">
-        <v>7.894736842105263</v>
+        <v>68.42105263157895</v>
       </c>
       <c r="E11">
         <v>76</v>
@@ -18681,10 +18681,10 @@
         <v>25</v>
       </c>
       <c r="C12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D12">
-        <v>3.79746835443038</v>
+        <v>5.063291139240507</v>
       </c>
       <c r="E12">
         <v>79</v>
@@ -18698,10 +18698,10 @@
         <v>27</v>
       </c>
       <c r="C13">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="D13">
-        <v>6.578947368421052</v>
+        <v>40.78947368421053</v>
       </c>
       <c r="E13">
         <v>76</v>
@@ -18715,10 +18715,10 @@
         <v>29</v>
       </c>
       <c r="C14">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="D14">
-        <v>7.894736842105263</v>
+        <v>64.47368421052632</v>
       </c>
       <c r="E14">
         <v>76</v>
@@ -18732,10 +18732,10 @@
         <v>31</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="D15">
-        <v>2.631578947368421</v>
+        <v>34.21052631578947</v>
       </c>
       <c r="E15">
         <v>76</v>
@@ -18749,10 +18749,10 @@
         <v>33</v>
       </c>
       <c r="C16">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="D16">
-        <v>3.947368421052631</v>
+        <v>46.05263157894737</v>
       </c>
       <c r="E16">
         <v>76</v>
@@ -18766,10 +18766,10 @@
         <v>35</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D17">
-        <v>3.947368421052631</v>
+        <v>13.1578947368421</v>
       </c>
       <c r="E17">
         <v>76</v>
@@ -18783,10 +18783,10 @@
         <v>35</v>
       </c>
       <c r="C18">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="D18">
-        <v>3.947368421052631</v>
+        <v>38.15789473684211</v>
       </c>
       <c r="E18">
         <v>76</v>
@@ -18800,10 +18800,10 @@
         <v>38</v>
       </c>
       <c r="C19">
-        <v>5</v>
+        <v>70</v>
       </c>
       <c r="D19">
-        <v>6.578947368421052</v>
+        <v>92.10526315789474</v>
       </c>
       <c r="E19">
         <v>76</v>
@@ -18817,10 +18817,10 @@
         <v>40</v>
       </c>
       <c r="C20">
-        <v>5</v>
+        <v>75</v>
       </c>
       <c r="D20">
-        <v>6.578947368421052</v>
+        <v>98.68421052631578</v>
       </c>
       <c r="E20">
         <v>76</v>
@@ -18834,10 +18834,10 @@
         <v>19</v>
       </c>
       <c r="C21">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="D21">
-        <v>3.947368421052631</v>
+        <v>34.21052631578947</v>
       </c>
       <c r="E21">
         <v>76</v>
@@ -18851,10 +18851,10 @@
         <v>38</v>
       </c>
       <c r="C22">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D22">
-        <v>3.947368421052631</v>
+        <v>17.10526315789474</v>
       </c>
       <c r="E22">
         <v>76</v>
@@ -18868,10 +18868,10 @@
         <v>12</v>
       </c>
       <c r="C23">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="D23">
-        <v>2.631578947368421</v>
+        <v>44.73684210526316</v>
       </c>
       <c r="E23">
         <v>76</v>
@@ -18885,10 +18885,10 @@
         <v>6</v>
       </c>
       <c r="C24">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="D24">
-        <v>10.12658227848101</v>
+        <v>59.49367088607595</v>
       </c>
       <c r="E24">
         <v>79</v>
@@ -18902,10 +18902,10 @@
         <v>33</v>
       </c>
       <c r="C25">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="D25">
-        <v>7.894736842105263</v>
+        <v>63.1578947368421</v>
       </c>
       <c r="E25">
         <v>76</v>
@@ -18936,10 +18936,10 @@
         <v>49</v>
       </c>
       <c r="C27">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="D27">
-        <v>2.631578947368421</v>
+        <v>40.78947368421053</v>
       </c>
       <c r="E27">
         <v>76</v>
@@ -18953,10 +18953,10 @@
         <v>16</v>
       </c>
       <c r="C28">
-        <v>6</v>
+        <v>70</v>
       </c>
       <c r="D28">
-        <v>7.894736842105263</v>
+        <v>92.10526315789474</v>
       </c>
       <c r="E28">
         <v>76</v>
@@ -18970,10 +18970,10 @@
         <v>40</v>
       </c>
       <c r="C29">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="D29">
-        <v>3.947368421052631</v>
+        <v>71.05263157894737</v>
       </c>
       <c r="E29">
         <v>76</v>
@@ -18987,10 +18987,10 @@
         <v>53</v>
       </c>
       <c r="C30">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="D30">
-        <v>5.063291139240507</v>
+        <v>69.62025316455697</v>
       </c>
       <c r="E30">
         <v>79</v>
@@ -19004,10 +19004,10 @@
         <v>31</v>
       </c>
       <c r="C31">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D31">
-        <v>2.631578947368421</v>
+        <v>10.52631578947368</v>
       </c>
       <c r="E31">
         <v>76</v>
@@ -19021,10 +19021,10 @@
         <v>16</v>
       </c>
       <c r="C32">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="D32">
-        <v>3.947368421052631</v>
+        <v>46.05263157894737</v>
       </c>
       <c r="E32">
         <v>76</v>
@@ -19038,10 +19038,10 @@
         <v>19</v>
       </c>
       <c r="C33">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="D33">
-        <v>6.578947368421052</v>
+        <v>47.36842105263158</v>
       </c>
       <c r="E33">
         <v>76</v>
@@ -19055,10 +19055,10 @@
         <v>49</v>
       </c>
       <c r="C34">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="D34">
-        <v>2.631578947368421</v>
+        <v>47.36842105263158</v>
       </c>
       <c r="E34">
         <v>76</v>
@@ -19089,10 +19089,10 @@
         <v>61</v>
       </c>
       <c r="C36">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="D36">
-        <v>2.631578947368421</v>
+        <v>43.42105263157895</v>
       </c>
       <c r="E36">
         <v>76</v>
@@ -19106,10 +19106,10 @@
         <v>6</v>
       </c>
       <c r="C37">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="D37">
-        <v>12.65822784810127</v>
+        <v>59.49367088607595</v>
       </c>
       <c r="E37">
         <v>79</v>
@@ -19123,10 +19123,10 @@
         <v>8</v>
       </c>
       <c r="C38">
-        <v>5</v>
+        <v>75</v>
       </c>
       <c r="D38">
-        <v>6.578947368421052</v>
+        <v>98.68421052631578</v>
       </c>
       <c r="E38">
         <v>76</v>
@@ -19157,10 +19157,10 @@
         <v>21</v>
       </c>
       <c r="C40">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="D40">
-        <v>3.79746835443038</v>
+        <v>25.31645569620253</v>
       </c>
       <c r="E40">
         <v>79</v>
@@ -19174,10 +19174,10 @@
         <v>33</v>
       </c>
       <c r="C41">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="D41">
-        <v>11.84210526315789</v>
+        <v>64.47368421052632</v>
       </c>
       <c r="E41">
         <v>76</v>
@@ -19191,10 +19191,10 @@
         <v>14</v>
       </c>
       <c r="C42">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="D42">
-        <v>2.631578947368421</v>
+        <v>36.84210526315789</v>
       </c>
       <c r="E42">
         <v>76</v>
@@ -19208,10 +19208,10 @@
         <v>29</v>
       </c>
       <c r="C43">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="D43">
-        <v>6.578947368421052</v>
+        <v>75</v>
       </c>
       <c r="E43">
         <v>76</v>
@@ -19225,10 +19225,10 @@
         <v>8</v>
       </c>
       <c r="C44">
-        <v>3</v>
+        <v>68</v>
       </c>
       <c r="D44">
-        <v>3.947368421052631</v>
+        <v>89.47368421052632</v>
       </c>
       <c r="E44">
         <v>76</v>
@@ -19242,10 +19242,10 @@
         <v>49</v>
       </c>
       <c r="C45">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="D45">
-        <v>2.631578947368421</v>
+        <v>34.21052631578947</v>
       </c>
       <c r="E45">
         <v>76</v>
@@ -19259,10 +19259,10 @@
         <v>40</v>
       </c>
       <c r="C46">
-        <v>5</v>
+        <v>64</v>
       </c>
       <c r="D46">
-        <v>6.578947368421052</v>
+        <v>84.21052631578947</v>
       </c>
       <c r="E46">
         <v>76</v>
@@ -19276,10 +19276,10 @@
         <v>23</v>
       </c>
       <c r="C47">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D47">
-        <v>3.947368421052631</v>
+        <v>19.73684210526316</v>
       </c>
       <c r="E47">
         <v>76</v>
@@ -19293,10 +19293,10 @@
         <v>16</v>
       </c>
       <c r="C48">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="D48">
-        <v>5.263157894736842</v>
+        <v>48.68421052631579</v>
       </c>
       <c r="E48">
         <v>76</v>
@@ -19310,10 +19310,10 @@
         <v>75</v>
       </c>
       <c r="C49">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="D49">
-        <v>10.52631578947368</v>
+        <v>47.36842105263158</v>
       </c>
       <c r="E49">
         <v>76</v>
@@ -19327,10 +19327,10 @@
         <v>77</v>
       </c>
       <c r="C50">
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="D50">
-        <v>2.631578947368421</v>
+        <v>61.8421052631579</v>
       </c>
       <c r="E50">
         <v>76</v>
@@ -19344,10 +19344,10 @@
         <v>12</v>
       </c>
       <c r="C51">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="D51">
-        <v>2.631578947368421</v>
+        <v>44.73684210526316</v>
       </c>
       <c r="E51">
         <v>76</v>
@@ -19361,10 +19361,10 @@
         <v>6</v>
       </c>
       <c r="C52">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="D52">
-        <v>11.39240506329114</v>
+        <v>49.36708860759494</v>
       </c>
       <c r="E52">
         <v>79</v>
@@ -19378,10 +19378,10 @@
         <v>21</v>
       </c>
       <c r="C53">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D53">
-        <v>3.79746835443038</v>
+        <v>13.92405063291139</v>
       </c>
       <c r="E53">
         <v>79</v>
@@ -19395,10 +19395,10 @@
         <v>61</v>
       </c>
       <c r="C54">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D54">
-        <v>2.631578947368421</v>
+        <v>28.94736842105263</v>
       </c>
       <c r="E54">
         <v>76</v>
@@ -19412,10 +19412,10 @@
         <v>40</v>
       </c>
       <c r="C55">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="D55">
-        <v>5.263157894736842</v>
+        <v>75</v>
       </c>
       <c r="E55">
         <v>76</v>
@@ -19429,10 +19429,10 @@
         <v>84</v>
       </c>
       <c r="C56">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="D56">
-        <v>2.631578947368421</v>
+        <v>25</v>
       </c>
       <c r="E56">
         <v>76</v>
@@ -19446,10 +19446,10 @@
         <v>38</v>
       </c>
       <c r="C57">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="D57">
-        <v>3.947368421052631</v>
+        <v>71.05263157894737</v>
       </c>
       <c r="E57">
         <v>76</v>
@@ -19463,10 +19463,10 @@
         <v>49</v>
       </c>
       <c r="C58">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="D58">
-        <v>3.947368421052631</v>
+        <v>46.05263157894737</v>
       </c>
       <c r="E58">
         <v>76</v>
@@ -19480,10 +19480,10 @@
         <v>14</v>
       </c>
       <c r="C59">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="D59">
-        <v>2.631578947368421</v>
+        <v>36.84210526315789</v>
       </c>
       <c r="E59">
         <v>76</v>
@@ -19497,10 +19497,10 @@
         <v>19</v>
       </c>
       <c r="C60">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="D60">
-        <v>3.947368421052631</v>
+        <v>40.78947368421053</v>
       </c>
       <c r="E60">
         <v>76</v>
@@ -19531,10 +19531,10 @@
         <v>49</v>
       </c>
       <c r="C62">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="D62">
-        <v>2.631578947368421</v>
+        <v>40.78947368421053</v>
       </c>
       <c r="E62">
         <v>76</v>
@@ -19548,10 +19548,10 @@
         <v>35</v>
       </c>
       <c r="C63">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="D63">
-        <v>2.631578947368421</v>
+        <v>36.84210526315789</v>
       </c>
       <c r="E63">
         <v>76</v>
@@ -19565,10 +19565,10 @@
         <v>19</v>
       </c>
       <c r="C64">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="D64">
-        <v>3.947368421052631</v>
+        <v>23.68421052631579</v>
       </c>
       <c r="E64">
         <v>76</v>
@@ -19582,10 +19582,10 @@
         <v>19</v>
       </c>
       <c r="C65">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="D65">
-        <v>2.631578947368421</v>
+        <v>36.84210526315789</v>
       </c>
       <c r="E65">
         <v>76</v>
@@ -19599,10 +19599,10 @@
         <v>38</v>
       </c>
       <c r="C66">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="D66">
-        <v>3.947368421052631</v>
+        <v>48.68421052631579</v>
       </c>
       <c r="E66">
         <v>76</v>
@@ -19616,10 +19616,10 @@
         <v>19</v>
       </c>
       <c r="C67">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="D67">
-        <v>5.263157894736842</v>
+        <v>47.36842105263158</v>
       </c>
       <c r="E67">
         <v>76</v>
@@ -19633,10 +19633,10 @@
         <v>49</v>
       </c>
       <c r="C68">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="D68">
-        <v>2.631578947368421</v>
+        <v>36.84210526315789</v>
       </c>
       <c r="E68">
         <v>76</v>
@@ -19667,10 +19667,10 @@
         <v>77</v>
       </c>
       <c r="C70">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="D70">
-        <v>3.947368421052631</v>
+        <v>71.05263157894737</v>
       </c>
       <c r="E70">
         <v>76</v>
@@ -19684,10 +19684,10 @@
         <v>98</v>
       </c>
       <c r="C71">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D71">
-        <v>1.31578947368421</v>
+        <v>13.1578947368421</v>
       </c>
       <c r="E71">
         <v>76</v>
@@ -19701,10 +19701,10 @@
         <v>23</v>
       </c>
       <c r="C72">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="D72">
-        <v>7.894736842105263</v>
+        <v>72.36842105263158</v>
       </c>
       <c r="E72">
         <v>76</v>
@@ -19718,10 +19718,10 @@
         <v>35</v>
       </c>
       <c r="C73">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D73">
-        <v>2.631578947368421</v>
+        <v>3.947368421052631</v>
       </c>
       <c r="E73">
         <v>76</v>
@@ -19735,10 +19735,10 @@
         <v>14</v>
       </c>
       <c r="C74">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D74">
-        <v>2.631578947368421</v>
+        <v>21.05263157894737</v>
       </c>
       <c r="E74">
         <v>76</v>

</xml_diff>